<commit_message>
Integrate all functions in main shell, etc
1. All functions that were in shell/src were integrated into
   shell/execution.sh. In accordance with this revision, the 2 future
   simulation functions were integrated into one.
2. The activation of loading settings by declaring different setting
   shell file. If not specified, the original setting
   (shell/settings.sh) is loaded.
3. Small revisions for the better code readability.

2022/3/10 Katsuya Sasaki
</commit_message>
<xml_diff>
--- a/define/inc_shell/scenario_settings.xlsx
+++ b/define/inc_shell/scenario_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ksasaki\research\tekito\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ksasaki\research\AIMPLUM\model\define\inc_shell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{461708EF-776E-46FF-A037-863F9597952F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71337636-C98B-4ABF-AAEC-E2EBF389E6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kari" sheetId="1" r:id="rId1"/>
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,7 +487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,6 +665,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -912,8 +918,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1270,26 +1279,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>